<commit_message>
Antes de fazer algumas alterações ousadas
</commit_message>
<xml_diff>
--- a/First_Follow_Tabela.xlsx
+++ b/First_Follow_Tabela.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tadio\OneDrive\Área de Trabalho\Facul\COMP\Compilador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34CAAD2-29E5-4F3B-BF44-BE8FF40AB5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42726E69-55F5-4FF6-B135-57894DAE4BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A2150D8B-7879-4D64-BED4-E4133F5879B3}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{A2150D8B-7879-4D64-BED4-E4133F5879B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -1155,7 +1155,7 @@
   <dimension ref="A1:AI30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2604,23 +2604,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="97651425-3362-4ddf-9ec3-4160ff4b44c4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010029E7B0A34555DE40A5A0426AAA539669" ma:contentTypeVersion="16" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="c51c33a3a94dba8123cb3ff5cc6f7340">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="97651425-3362-4ddf-9ec3-4160ff4b44c4" xmlns:ns4="6707ad17-fd97-45ac-870d-7d22539aa422" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66c557ebdaf3404c806ff522a247f990" ns3:_="" ns4:_="">
     <xsd:import namespace="97651425-3362-4ddf-9ec3-4160ff4b44c4"/>
@@ -2861,10 +2844,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="97651425-3362-4ddf-9ec3-4160ff4b44c4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D38FDB-1564-4AD3-8645-DAB9058AC7DC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D22D67F-E99E-4950-A077-EE5D308C4995}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="97651425-3362-4ddf-9ec3-4160ff4b44c4"/>
+    <ds:schemaRef ds:uri="6707ad17-fd97-45ac-870d-7d22539aa422"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2887,20 +2898,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D22D67F-E99E-4950-A077-EE5D308C4995}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D38FDB-1564-4AD3-8645-DAB9058AC7DC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="97651425-3362-4ddf-9ec3-4160ff4b44c4"/>
-    <ds:schemaRef ds:uri="6707ad17-fd97-45ac-870d-7d22539aa422"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
No meio do concerto
</commit_message>
<xml_diff>
--- a/First_Follow_Tabela.xlsx
+++ b/First_Follow_Tabela.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tadio\OneDrive\Área de Trabalho\Facul\COMP\Compilador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42726E69-55F5-4FF6-B135-57894DAE4BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320EE530-58D2-430D-BCF9-4FFB01D41CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{A2150D8B-7879-4D64-BED4-E4133F5879B3}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{A2150D8B-7879-4D64-BED4-E4133F5879B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="136">
   <si>
     <t>Simbolo</t>
   </si>
@@ -89,12 +89,6 @@
     <t>ConteudoDO</t>
   </si>
   <si>
-    <t>ConteudoWhile</t>
-  </si>
-  <si>
-    <t>ConteudoWhile'</t>
-  </si>
-  <si>
     <t>ConteudoCondicao</t>
   </si>
   <si>
@@ -182,9 +176,6 @@
     <t>par_dir, $, col_dir</t>
   </si>
   <si>
-    <t>fim_linha, else, par_dir, virgula, $, col_dir</t>
-  </si>
-  <si>
     <t>col_dir</t>
   </si>
   <si>
@@ -362,12 +353,6 @@
     <t>&lt;ConteudoDO&gt;:=col_esq&lt;program&gt;col_dir</t>
   </si>
   <si>
-    <t>AuxConteudoWhile</t>
-  </si>
-  <si>
-    <t>op_relacional, fim_linha</t>
-  </si>
-  <si>
     <t>&lt;ConteudoWhile&gt;:=id&lt;AuxConteudoWhile&gt;</t>
   </si>
   <si>
@@ -435,6 +420,30 @@
   </si>
   <si>
     <t>&lt;Increm_decrem&gt;:=decremento</t>
+  </si>
+  <si>
+    <t>ConteudoCondicaoWhile</t>
+  </si>
+  <si>
+    <t>ConteudoCondicaoWhile'</t>
+  </si>
+  <si>
+    <t>op_relacional, op_aritmetico, or, and, fim_linha</t>
+  </si>
+  <si>
+    <t>ConteudoCondicaoFor</t>
+  </si>
+  <si>
+    <t>ConteudoCondicaoFor'</t>
+  </si>
+  <si>
+    <t>op_relacional, op_aritmetico, or, and, virgula</t>
+  </si>
+  <si>
+    <t>fim_linha, else, par_dir</t>
+  </si>
+  <si>
+    <t>id, par_dir</t>
   </si>
 </sst>
 </file>
@@ -464,12 +473,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="21">
@@ -618,16 +633,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -637,19 +650,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -727,6 +727,21 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -744,7 +759,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -788,34 +803,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1154,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA08CFE-D3E1-4620-88B7-74C5EB954786}">
   <dimension ref="A1:AI30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,8 +1188,8 @@
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="2" max="2" width="51.85546875" customWidth="1"/>
     <col min="3" max="3" width="45.140625" customWidth="1"/>
-    <col min="4" max="4" width="4" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="5" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
     <col min="6" max="6" width="51.42578125" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
     <col min="8" max="8" width="41.7109375" customWidth="1"/>
@@ -1207,122 +1232,122 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>43</v>
+      <c r="B2" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="F2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="F2" s="16" t="s">
+      <c r="J2" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="19" t="s">
+      <c r="R2" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="M2" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="19" t="s">
+      <c r="S2" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="O2" s="19" t="s">
+      <c r="T2" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="P2" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" s="19" t="s">
+      <c r="U2" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="S2" s="19" t="s">
+      <c r="V2" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="T2" s="19" t="s">
+      <c r="W2" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="U2" s="19" t="s">
+      <c r="X2" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="V2" s="19" t="s">
+      <c r="Y2" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="W2" s="19" t="s">
+      <c r="Z2" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="X2" s="19" t="s">
+      <c r="AA2" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB2" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="Y2" s="19" t="s">
+      <c r="AC2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD2" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="Z2" s="19" t="s">
+      <c r="AE2" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="AA2" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB2" s="19" t="s">
+      <c r="AF2" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="AC2" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD2" s="19" t="s">
+      <c r="AG2" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="AE2" s="19" t="s">
+      <c r="AH2" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="AF2" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG2" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="AH2" s="20" t="s">
+      <c r="AI2" s="23" t="s">
         <v>68</v>
-      </c>
-      <c r="AI2" s="24" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>42</v>
+      <c r="B3" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="17"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1333,59 +1358,59 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
       <c r="AC3" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="AD3" s="4"/>
       <c r="AE3" s="4"/>
       <c r="AF3" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AG3" s="4"/>
       <c r="AH3" s="8"/>
       <c r="AI3" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>32</v>
+      <c r="B4" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="15"/>
+      <c r="F4" s="14"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -1400,16 +1425,16 @@
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="W4" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="W4" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
@@ -1425,20 +1450,20 @@
       <c r="AI4" s="5"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>80</v>
+      <c r="A5" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="14"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -1449,7 +1474,7 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
@@ -1472,25 +1497,25 @@
       <c r="AI5" s="5"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>34</v>
+      <c r="B6" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" s="15"/>
+        <v>75</v>
+      </c>
+      <c r="F6" s="14"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -1501,7 +1526,7 @@
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
@@ -1521,21 +1546,21 @@
       <c r="AI6" s="5"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>41</v>
+      <c r="B7" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="15" t="s">
-        <v>83</v>
+      <c r="F7" s="14" t="s">
+        <v>80</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1545,16 +1570,16 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="P7" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="O7" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="Q7" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
@@ -1576,44 +1601,44 @@
       <c r="AI7" s="5"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>38</v>
+      <c r="B8" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>88</v>
+      <c r="F8" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
@@ -1635,20 +1660,20 @@
       <c r="AI8" s="5"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>92</v>
+      <c r="A9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="15"/>
+      <c r="F9" s="14"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -1662,7 +1687,7 @@
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
       <c r="S9" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
@@ -1681,21 +1706,21 @@
       <c r="AI9" s="5"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>25</v>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
@@ -1705,16 +1730,16 @@
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
@@ -1726,7 +1751,7 @@
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
       <c r="AA10" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AB10" s="10"/>
       <c r="AC10" s="10"/>
@@ -1738,25 +1763,25 @@
       <c r="AI10" s="10"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>26</v>
+      <c r="B11" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="15"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -1785,20 +1810,20 @@
       <c r="AI11" s="5"/>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>27</v>
+      <c r="B12" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="23"/>
+      <c r="F12" s="22"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1820,7 +1845,7 @@
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
       <c r="AA12" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="AB12" s="4"/>
       <c r="AC12" s="4"/>
@@ -1832,21 +1857,21 @@
       <c r="AI12" s="4"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>28</v>
+      <c r="B13" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="15" t="s">
-        <v>98</v>
+      <c r="F13" s="14" t="s">
+        <v>95</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -1878,20 +1903,20 @@
       <c r="AI13" s="5"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>27</v>
+      <c r="B14" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="15"/>
+      <c r="F14" s="14"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -1915,7 +1940,7 @@
       <c r="AA14" s="5"/>
       <c r="AB14" s="5"/>
       <c r="AC14" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
@@ -1925,21 +1950,21 @@
       <c r="AI14" s="5"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>101</v>
+      <c r="B15" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="15" t="s">
-        <v>100</v>
+      <c r="F15" s="14" t="s">
+        <v>97</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -1972,20 +1997,20 @@
       <c r="AI15" s="5"/>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>30</v>
+      <c r="B16" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="15"/>
+      <c r="F16" s="14"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
@@ -1996,10 +2021,10 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Q16" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
@@ -2021,20 +2046,20 @@
       <c r="AI16" s="5"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>31</v>
+      <c r="B17" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="15"/>
+      <c r="F17" s="14"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -2055,40 +2080,40 @@
       <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
       <c r="Z17" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="AA17" s="5"/>
       <c r="AB17" s="5"/>
       <c r="AC17" s="5"/>
       <c r="AD17" s="5"/>
       <c r="AE17" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="AF17" s="5"/>
       <c r="AG17" s="5"/>
       <c r="AH17" s="2"/>
       <c r="AI17" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="7" t="s">
+      <c r="A18" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="15"/>
+      <c r="F18" s="14"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -2119,19 +2144,19 @@
       <c r="AI18" s="5"/>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>109</v>
+      <c r="A19" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="15"/>
+        <v>135</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="F19" s="14"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -2142,7 +2167,7 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
@@ -2165,29 +2190,29 @@
       <c r="AI19" s="5"/>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>33</v>
+      <c r="A20" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="F20" s="15"/>
+        <v>44</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="F20" s="14"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
@@ -2213,19 +2238,19 @@
       <c r="AI20" s="5"/>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>34</v>
+      <c r="A21" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="15"/>
+        <v>134</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="F21" s="14"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -2233,7 +2258,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
@@ -2259,20 +2284,20 @@
       <c r="AI21" s="5"/>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>35</v>
+      <c r="A22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>48</v>
+        <v>134</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>118</v>
+        <v>17</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -2282,16 +2307,16 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
       <c r="N22" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="Q22" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
@@ -2313,31 +2338,31 @@
       <c r="AI22" s="5"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>37</v>
+      <c r="A23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" s="15"/>
+        <v>34</v>
+      </c>
+      <c r="F23" s="14"/>
       <c r="G23" s="5"/>
       <c r="H23" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
@@ -2354,11 +2379,11 @@
       <c r="Z23" s="5"/>
       <c r="AA23" s="5"/>
       <c r="AB23" s="5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="AC23" s="5"/>
       <c r="AD23" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="AE23" s="5"/>
       <c r="AF23" s="5"/>
@@ -2367,24 +2392,24 @@
       <c r="AI23" s="5"/>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>32</v>
+      <c r="A24" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="15"/>
+        <v>18</v>
+      </c>
+      <c r="F24" s="14"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
@@ -2406,7 +2431,7 @@
       <c r="AC24" s="5"/>
       <c r="AD24" s="5"/>
       <c r="AE24" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="AF24" s="5"/>
       <c r="AG24" s="5"/>
@@ -2414,19 +2439,19 @@
       <c r="AI24" s="5"/>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>38</v>
+      <c r="A25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" s="15"/>
+        <v>19</v>
+      </c>
+      <c r="F25" s="14"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -2437,7 +2462,7 @@
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
@@ -2460,19 +2485,19 @@
       <c r="AI25" s="5"/>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>39</v>
+      <c r="A26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="15"/>
+        <v>20</v>
+      </c>
+      <c r="F26" s="14"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -2486,7 +2511,7 @@
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
       <c r="S26" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="T26" s="5"/>
       <c r="U26" s="5"/>
@@ -2506,19 +2531,19 @@
       <c r="AI26" s="5"/>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>31</v>
+      <c r="A27" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="15"/>
+        <v>21</v>
+      </c>
+      <c r="F27" s="14"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -2527,13 +2552,13 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="O27" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="P27" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
@@ -2556,10 +2581,19 @@
       <c r="AI27" s="5"/>
     </row>
     <row r="28" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E28" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28" s="15"/>
+      <c r="A28" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="14"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -2578,10 +2612,10 @@
       <c r="V28" s="5"/>
       <c r="W28" s="5"/>
       <c r="X28" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="Y28" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="Z28" s="5"/>
       <c r="AA28" s="5"/>
@@ -2594,6 +2628,43 @@
       <c r="AH28" s="2"/>
       <c r="AI28" s="5"/>
     </row>
+    <row r="29" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="E29" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="F29" s="26"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="25"/>
+      <c r="N29" s="25"/>
+      <c r="O29" s="25"/>
+      <c r="P29" s="25"/>
+      <c r="Q29" s="25"/>
+      <c r="R29" s="25"/>
+      <c r="S29" s="25"/>
+      <c r="T29" s="25"/>
+      <c r="U29" s="25"/>
+      <c r="V29" s="25"/>
+      <c r="W29" s="25"/>
+      <c r="X29" s="25"/>
+      <c r="Y29" s="25"/>
+      <c r="Z29" s="25"/>
+      <c r="AA29" s="25"/>
+      <c r="AB29" s="25"/>
+      <c r="AC29" s="25"/>
+      <c r="AD29" s="25"/>
+      <c r="AE29" s="25"/>
+      <c r="AF29" s="25"/>
+      <c r="AG29" s="25"/>
+      <c r="AH29" s="25"/>
+      <c r="AI29" s="25"/>
+    </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B30" s="9"/>
     </row>
@@ -2604,6 +2675,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="97651425-3362-4ddf-9ec3-4160ff4b44c4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010029E7B0A34555DE40A5A0426AAA539669" ma:contentTypeVersion="16" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="c51c33a3a94dba8123cb3ff5cc6f7340">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="97651425-3362-4ddf-9ec3-4160ff4b44c4" xmlns:ns4="6707ad17-fd97-45ac-870d-7d22539aa422" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66c557ebdaf3404c806ff522a247f990" ns3:_="" ns4:_="">
     <xsd:import namespace="97651425-3362-4ddf-9ec3-4160ff4b44c4"/>
@@ -2844,38 +2932,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="97651425-3362-4ddf-9ec3-4160ff4b44c4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D22D67F-E99E-4950-A077-EE5D308C4995}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D38FDB-1564-4AD3-8645-DAB9058AC7DC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="97651425-3362-4ddf-9ec3-4160ff4b44c4"/>
-    <ds:schemaRef ds:uri="6707ad17-fd97-45ac-870d-7d22539aa422"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2898,9 +2958,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D38FDB-1564-4AD3-8645-DAB9058AC7DC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D22D67F-E99E-4950-A077-EE5D308C4995}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="97651425-3362-4ddf-9ec3-4160ff4b44c4"/>
+    <ds:schemaRef ds:uri="6707ad17-fd97-45ac-870d-7d22539aa422"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Algumas coisas foram arrumadas
</commit_message>
<xml_diff>
--- a/First_Follow_Tabela.xlsx
+++ b/First_Follow_Tabela.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tadio\OneDrive\Área de Trabalho\Facul\COMP\Compilador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320EE530-58D2-430D-BCF9-4FFB01D41CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3831690-B2F0-47AB-8939-CCFBF5F54A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{A2150D8B-7879-4D64-BED4-E4133F5879B3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A2150D8B-7879-4D64-BED4-E4133F5879B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="152">
   <si>
     <t>Simbolo</t>
   </si>
@@ -341,9 +341,6 @@
     <t>&lt;ConteúdoSaida&gt;:=string</t>
   </si>
   <si>
-    <t>&lt;LacoECondicao:=do&lt;ConteudoDO&gt;&lt;ConteudoWhile&gt;</t>
-  </si>
-  <si>
     <t>&lt;LacoECondicao:=if&lt;ConteudoCondicao&gt;</t>
   </si>
   <si>
@@ -353,18 +350,6 @@
     <t>&lt;ConteudoDO&gt;:=col_esq&lt;program&gt;col_dir</t>
   </si>
   <si>
-    <t>&lt;ConteudoWhile&gt;:=id&lt;AuxConteudoWhile&gt;</t>
-  </si>
-  <si>
-    <t>&lt;AuxConteudoWhile&gt;:=&lt;ConteudoWhile'&gt;</t>
-  </si>
-  <si>
-    <t>&lt;AuxConteudoWhile&gt;:=&lt;FimLinha&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ConteudoWhile'&gt;:=op_relacional&lt;Dados&gt;</t>
-  </si>
-  <si>
     <t>&lt;ConteudoCondicao&gt;:=string&lt;ConteudoCondicao’&gt;</t>
   </si>
   <si>
@@ -401,9 +386,6 @@
     <t>&lt;FinalCond&gt;:=else col_esq&lt;program&gt;col_dir fim_linha</t>
   </si>
   <si>
-    <t>&lt;ConteudoFor&gt; := id&lt;ValorInicial&gt;virgula&lt;ConteudoCondicao&gt; virgula id &lt;Increm_decrem&gt; col_esq &lt;program&gt; col_dir</t>
-  </si>
-  <si>
     <t>&lt;ValorInicial&gt;:=atribuição&lt;DadosAtrib&gt;</t>
   </si>
   <si>
@@ -444,6 +426,72 @@
   </si>
   <si>
     <t>id, par_dir</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoFor&gt; := id&lt;ValorInicial&gt;virgula&lt;ConteudoCondicaoFor&gt; id &lt;Increm_decrem&gt; col_esq &lt;program&gt; col_dir</t>
+  </si>
+  <si>
+    <t>&lt;LacoECondicao:=do&lt;ConteudoDO&gt;while&lt;ConteudoCondicaoWhile&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoWhile&gt;:=id&lt;ConteudoCondicaoWhile'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoWhile&gt;:=string&lt;ConteudoCondicaoWhile'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoWhile&gt;:=int&lt;ConteudoCondicaoWhile'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoWhile&gt;:=float&lt;ConteudoCondicaoWhile'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoWhile&gt;:=par_esq &lt;ConteudoCondicaoWhile&gt;par_dir</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoFor&gt;:=int&lt;ConteudoCondicaoFor'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoFor&gt;:=float&lt;ConteudoCondicaoFor'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoFor&gt;:=id&lt;ConteudoCondicaoFor'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoFor&gt;:=string&lt;ConteudoCondicaoFor'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoWhile'&gt;:=or &lt;ConteudoCondicaoWhile&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoWhile'&gt;:=and &lt;ConteudoCondicaoWhile&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoWhile'&gt;:=fim_linha</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoWhile'&gt;:=op_aritmetico&lt;ConteudoCondicaoWhile&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoWhile'&gt;:=op_relacional&lt;ConteudoCondicaoWhile&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoFor'&gt;:=op_aritmetico&lt;ConteudoCondicaoFor&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoFor'&gt;:=op_relacional&lt;ConteudoCondicaoFor&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoFor'&gt;:=or&lt;ConteudoCondicaoFor&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoFor'&gt;:=and&lt;ConteudoCondicaoFor&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoFor'&gt;:=virgula</t>
+  </si>
+  <si>
+    <t>&lt;ConteudoCondicaoFor&gt;:=par_esq &lt;ConteudoCondicaoFor&gt; par_dir</t>
   </si>
 </sst>
 </file>
@@ -759,7 +807,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -827,22 +875,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1177,10 +1222,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA08CFE-D3E1-4620-88B7-74C5EB954786}">
-  <dimension ref="A1:AI30"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,7 +1234,7 @@
     <col min="2" max="2" width="51.85546875" customWidth="1"/>
     <col min="3" max="3" width="45.140625" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
     <col min="6" max="6" width="51.42578125" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
     <col min="8" max="8" width="41.7109375" customWidth="1"/>
@@ -1211,13 +1256,14 @@
     <col min="28" max="28" width="40.7109375" customWidth="1"/>
     <col min="29" max="29" width="40.85546875" customWidth="1"/>
     <col min="30" max="30" width="41.7109375" customWidth="1"/>
-    <col min="31" max="31" width="44.85546875" customWidth="1"/>
-    <col min="32" max="32" width="27.5703125" customWidth="1"/>
+    <col min="31" max="31" width="51.85546875" customWidth="1"/>
+    <col min="32" max="32" width="37.42578125" customWidth="1"/>
     <col min="33" max="34" width="23" customWidth="1"/>
     <col min="35" max="35" width="48.85546875" customWidth="1"/>
+    <col min="36" max="36" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1231,7 +1277,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
@@ -1329,11 +1375,14 @@
       <c r="AH2" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="AI2" s="23" t="s">
+      <c r="AI2" s="27" t="s">
         <v>68</v>
       </c>
+      <c r="AJ2" s="28" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -1395,8 +1444,9 @@
       <c r="AI3" s="4" t="s">
         <v>69</v>
       </c>
+      <c r="AJ3" s="29"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -1448,8 +1498,9 @@
       <c r="AG4" s="5"/>
       <c r="AH4" s="2"/>
       <c r="AI4" s="5"/>
+      <c r="AJ4" s="23"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>75</v>
       </c>
@@ -1495,8 +1546,9 @@
       <c r="AG5" s="5"/>
       <c r="AH5" s="2"/>
       <c r="AI5" s="5"/>
+      <c r="AJ5" s="23"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
@@ -1544,8 +1596,9 @@
       <c r="AG6" s="5"/>
       <c r="AH6" s="2"/>
       <c r="AI6" s="5"/>
+      <c r="AJ6" s="23"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1599,8 +1652,9 @@
       <c r="AG7" s="5"/>
       <c r="AH7" s="2"/>
       <c r="AI7" s="5"/>
+      <c r="AJ7" s="23"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
@@ -1658,8 +1712,9 @@
       <c r="AG8" s="5"/>
       <c r="AH8" s="2"/>
       <c r="AI8" s="5"/>
+      <c r="AJ8" s="23"/>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>88</v>
       </c>
@@ -1704,8 +1759,9 @@
       <c r="AG9" s="5"/>
       <c r="AH9" s="2"/>
       <c r="AI9" s="5"/>
+      <c r="AJ9" s="23"/>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
@@ -1761,8 +1817,9 @@
       <c r="AG10" s="10"/>
       <c r="AH10" s="11"/>
       <c r="AI10" s="10"/>
+      <c r="AJ10" s="23"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -1808,8 +1865,9 @@
       <c r="AG11" s="5"/>
       <c r="AH11" s="5"/>
       <c r="AI11" s="5"/>
+      <c r="AJ11" s="23"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
@@ -1855,8 +1913,9 @@
       <c r="AG12" s="4"/>
       <c r="AH12" s="8"/>
       <c r="AI12" s="4"/>
+      <c r="AJ12" s="23"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
@@ -1901,8 +1960,9 @@
       <c r="AG13" s="5"/>
       <c r="AH13" s="2"/>
       <c r="AI13" s="5"/>
+      <c r="AJ13" s="23"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
@@ -1948,8 +2008,9 @@
       <c r="AG14" s="5"/>
       <c r="AH14" s="2"/>
       <c r="AI14" s="5"/>
+      <c r="AJ14" s="23"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
@@ -1995,8 +2056,9 @@
       <c r="AG15" s="5"/>
       <c r="AH15" s="2"/>
       <c r="AI15" s="5"/>
+      <c r="AJ15" s="23"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
@@ -2044,8 +2106,9 @@
       <c r="AG16" s="5"/>
       <c r="AH16" s="2"/>
       <c r="AI16" s="5"/>
+      <c r="AJ16" s="23"/>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>16</v>
       </c>
@@ -2080,25 +2143,25 @@
       <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
       <c r="Z17" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AA17" s="5"/>
       <c r="AB17" s="5"/>
       <c r="AC17" s="5"/>
       <c r="AD17" s="5"/>
-      <c r="AE17" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="AF17" s="5"/>
+      <c r="AF17" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="AG17" s="5"/>
       <c r="AH17" s="2"/>
       <c r="AI17" s="5" t="s">
-        <v>101</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="AJ17" s="23"/>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>32</v>
@@ -2113,7 +2176,7 @@
       <c r="F18" s="14"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -2142,21 +2205,24 @@
       <c r="AG18" s="5"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="5"/>
+      <c r="AJ18" s="23"/>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E19" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="F19" s="14"/>
+        <v>129</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>136</v>
+      </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -2164,12 +2230,18 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
+      <c r="N19" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>135</v>
+      </c>
       <c r="P19" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q19" s="5"/>
+        <v>132</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>133</v>
+      </c>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
@@ -2188,36 +2260,43 @@
       <c r="AG19" s="5"/>
       <c r="AH19" s="2"/>
       <c r="AI19" s="5"/>
+      <c r="AJ19" s="23"/>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="F20" s="14"/>
+      <c r="E20" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>151</v>
+      </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="5" t="s">
-        <v>107</v>
-      </c>
+      <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="O20" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="P20" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q20" s="14" t="s">
+        <v>140</v>
+      </c>
       <c r="R20" s="5"/>
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
@@ -2236,8 +2315,9 @@
       <c r="AG20" s="5"/>
       <c r="AH20" s="2"/>
       <c r="AI20" s="5"/>
+      <c r="AJ20" s="23"/>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>17</v>
       </c>
@@ -2245,20 +2325,24 @@
         <v>32</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>123</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
+      <c r="J21" s="5" t="s">
+        <v>143</v>
+      </c>
       <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
+      <c r="L21" s="5" t="s">
+        <v>144</v>
+      </c>
       <c r="M21" s="5" t="s">
-        <v>108</v>
+        <v>145</v>
       </c>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
@@ -2274,16 +2358,21 @@
       <c r="Y21" s="5"/>
       <c r="Z21" s="5"/>
       <c r="AA21" s="5"/>
-      <c r="AB21" s="5"/>
+      <c r="AB21" s="5" t="s">
+        <v>141</v>
+      </c>
       <c r="AC21" s="5"/>
-      <c r="AD21" s="5"/>
+      <c r="AD21" s="5" t="s">
+        <v>142</v>
+      </c>
       <c r="AE21" s="5"/>
       <c r="AF21" s="5"/>
       <c r="AG21" s="5"/>
       <c r="AH21" s="2"/>
       <c r="AI21" s="5"/>
+      <c r="AJ21" s="23"/>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>34</v>
       </c>
@@ -2291,13 +2380,13 @@
         <v>33</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>17</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -2307,16 +2396,16 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
       <c r="N22" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="Q22" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
@@ -2336,8 +2425,9 @@
       <c r="AG22" s="5"/>
       <c r="AH22" s="2"/>
       <c r="AI22" s="5"/>
+      <c r="AJ22" s="23"/>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>18</v>
       </c>
@@ -2353,16 +2443,16 @@
       <c r="F23" s="14"/>
       <c r="G23" s="5"/>
       <c r="H23" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
@@ -2379,19 +2469,20 @@
       <c r="Z23" s="5"/>
       <c r="AA23" s="5"/>
       <c r="AB23" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="AC23" s="5"/>
       <c r="AD23" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="AE23" s="5"/>
       <c r="AF23" s="5"/>
       <c r="AG23" s="5"/>
       <c r="AH23" s="2"/>
       <c r="AI23" s="5"/>
+      <c r="AJ23" s="23"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>19</v>
       </c>
@@ -2409,7 +2500,7 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
@@ -2431,14 +2522,15 @@
       <c r="AC24" s="5"/>
       <c r="AD24" s="5"/>
       <c r="AE24" s="5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="AF24" s="5"/>
       <c r="AG24" s="5"/>
       <c r="AH24" s="2"/>
       <c r="AI24" s="5"/>
+      <c r="AJ24" s="23"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>20</v>
       </c>
@@ -2462,7 +2554,7 @@
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
@@ -2483,8 +2575,9 @@
       <c r="AG25" s="5"/>
       <c r="AH25" s="2"/>
       <c r="AI25" s="5"/>
+      <c r="AJ25" s="23"/>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>21</v>
       </c>
@@ -2511,7 +2604,7 @@
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
       <c r="S26" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="T26" s="5"/>
       <c r="U26" s="5"/>
@@ -2529,8 +2622,9 @@
       <c r="AG26" s="5"/>
       <c r="AH26" s="2"/>
       <c r="AI26" s="5"/>
+      <c r="AJ26" s="23"/>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>22</v>
       </c>
@@ -2552,13 +2646,13 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="O27" s="5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="P27" s="5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
@@ -2579,16 +2673,17 @@
       <c r="AG27" s="5"/>
       <c r="AH27" s="2"/>
       <c r="AI27" s="5"/>
+      <c r="AJ27" s="23"/>
     </row>
-    <row r="28" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="30" t="s">
-        <v>132</v>
+    <row r="28" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>135</v>
+        <v>127</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="E28" s="20" t="s">
         <v>22</v>
@@ -2612,10 +2707,10 @@
       <c r="V28" s="5"/>
       <c r="W28" s="5"/>
       <c r="X28" s="5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="Y28" s="5" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="Z28" s="5"/>
       <c r="AA28" s="5"/>
@@ -2627,45 +2722,55 @@
       <c r="AG28" s="5"/>
       <c r="AH28" s="2"/>
       <c r="AI28" s="5"/>
+      <c r="AJ28" s="23"/>
     </row>
-    <row r="29" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="E29" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="F29" s="26"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="25"/>
-      <c r="O29" s="25"/>
-      <c r="P29" s="25"/>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="25"/>
-      <c r="S29" s="25"/>
-      <c r="T29" s="25"/>
-      <c r="U29" s="25"/>
-      <c r="V29" s="25"/>
-      <c r="W29" s="25"/>
-      <c r="X29" s="25"/>
-      <c r="Y29" s="25"/>
-      <c r="Z29" s="25"/>
-      <c r="AA29" s="25"/>
-      <c r="AB29" s="25"/>
-      <c r="AC29" s="25"/>
-      <c r="AD29" s="25"/>
-      <c r="AE29" s="25"/>
-      <c r="AF29" s="25"/>
-      <c r="AG29" s="25"/>
-      <c r="AH29" s="25"/>
-      <c r="AI29" s="25"/>
+    <row r="29" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="F29" s="24"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="23"/>
+      <c r="U29" s="23"/>
+      <c r="V29" s="23"/>
+      <c r="W29" s="23"/>
+      <c r="X29" s="23"/>
+      <c r="Y29" s="23"/>
+      <c r="Z29" s="23"/>
+      <c r="AA29" s="23"/>
+      <c r="AB29" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC29" s="23"/>
+      <c r="AD29" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="AE29" s="23"/>
+      <c r="AF29" s="23"/>
+      <c r="AG29" s="23"/>
+      <c r="AH29" s="23"/>
+      <c r="AI29" s="23"/>
+      <c r="AJ29" s="23" t="s">
+        <v>150</v>
+      </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B30" s="9"/>
     </row>
   </sheetData>
@@ -2675,23 +2780,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="97651425-3362-4ddf-9ec3-4160ff4b44c4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010029E7B0A34555DE40A5A0426AAA539669" ma:contentTypeVersion="16" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="c51c33a3a94dba8123cb3ff5cc6f7340">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="97651425-3362-4ddf-9ec3-4160ff4b44c4" xmlns:ns4="6707ad17-fd97-45ac-870d-7d22539aa422" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66c557ebdaf3404c806ff522a247f990" ns3:_="" ns4:_="">
     <xsd:import namespace="97651425-3362-4ddf-9ec3-4160ff4b44c4"/>
@@ -2932,10 +3020,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="97651425-3362-4ddf-9ec3-4160ff4b44c4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D38FDB-1564-4AD3-8645-DAB9058AC7DC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D22D67F-E99E-4950-A077-EE5D308C4995}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="97651425-3362-4ddf-9ec3-4160ff4b44c4"/>
+    <ds:schemaRef ds:uri="6707ad17-fd97-45ac-870d-7d22539aa422"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2958,20 +3074,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D22D67F-E99E-4950-A077-EE5D308C4995}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D38FDB-1564-4AD3-8645-DAB9058AC7DC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="97651425-3362-4ddf-9ec3-4160ff4b44c4"/>
-    <ds:schemaRef ds:uri="6707ad17-fd97-45ac-870d-7d22539aa422"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>